<commit_message>
Update Excel template Samit new subject therapeutic tutoring, Sir rakaz
</commit_message>
<xml_diff>
--- a/CommitmentLettersApp/ImportTemplates/תבנית יבוא התחיבויות סאמיט.xlsx
+++ b/CommitmentLettersApp/ImportTemplates/תבנית יבוא התחיבויות סאמיט.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofir/Develop/Clients/DRLogy/Site/DrLogyMisc/CommitmentLettersApp/ImportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0153A6-DA7A-844E-8832-D33F169BDF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBC57BA-5E42-9D40-ABB1-F2EC5CAE3B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="13760" windowWidth="23200" windowHeight="10300" xr2:uid="{80D5FA03-17CC-472B-A333-F3A10A5D6810}"/>
+    <workbookView xWindow="3420" yWindow="4460" windowWidth="31660" windowHeight="18020" xr2:uid="{80D5FA03-17CC-472B-A333-F3A10A5D6810}"/>
   </bookViews>
   <sheets>
     <sheet name="ראשי" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>ת.ז</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>תרגום</t>
+  </si>
+  <si>
+    <t>חונכות טיפולית</t>
+  </si>
+  <si>
+    <t>שיר</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -752,7 +758,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54A042F5-6A70-4167-8F45-95036D4E9037}">
           <x14:formula1>
-            <xm:f>טבלאות!$C$2:$C$13</xm:f>
+            <xm:f>טבלאות!$C$2:$C$14</xm:f>
           </x14:formula1>
           <xm:sqref>L2</xm:sqref>
         </x14:dataValidation>
@@ -765,10 +771,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C62C1A-47BA-428A-A7F6-55A218332B22}">
   <sheetPr codeName="Worksheet______2"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C3" sqref="C3:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -797,7 +803,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
@@ -808,7 +814,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -819,18 +825,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
       <c r="C6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
@@ -863,6 +875,11 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>